<commit_message>
ESP32-S3 WROOM 2 hinzugefügt.
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christoph/Desktop/voltagerecorder-main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\voltagerecorder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C439AA2-8712-394B-B74E-DD2CCD1A1E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD0A250-6EBD-4EB6-9E9B-4B9B1CE12CE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="6460" windowWidth="14400" windowHeight="17500" xr2:uid="{48E2811D-28A7-1949-BAB9-61FD3C46DFFE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{48E2811D-28A7-1949-BAB9-61FD3C46DFFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Anzahl</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>MLFA1FTC4K70CT-ND</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710-830003000 </t>
+  </si>
+  <si>
+    <t>Crystal 32.786kHz</t>
   </si>
 </sst>
 </file>
@@ -155,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -171,7 +180,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -467,20 +476,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AF3DBB-0668-B84A-B00B-44B9FC9FC66A}">
-  <dimension ref="A8:D20"/>
+  <dimension ref="A8:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -494,7 +503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -505,7 +514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>6</v>
       </c>
@@ -516,7 +525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>8</v>
       </c>
@@ -527,7 +536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -538,7 +547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2</v>
       </c>
@@ -549,7 +558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>4</v>
       </c>
@@ -560,7 +569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -571,7 +580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3</v>
       </c>
@@ -582,7 +591,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -593,7 +602,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>9</v>
       </c>
@@ -604,7 +613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3</v>
       </c>
@@ -615,7 +624,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3</v>
       </c>
@@ -624,6 +633,22 @@
       </c>
       <c r="D20" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SD und USB-C added.
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\voltagerecorder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DCE604-68A0-442C-AC99-C8E9B04B44F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FECD51-2547-4EDA-AF8B-E94E464DFD70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{48E2811D-28A7-1949-BAB9-61FD3C46DFFE}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15290" xr2:uid="{48E2811D-28A7-1949-BAB9-61FD3C46DFFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Anzahl</t>
   </si>
@@ -130,7 +130,13 @@
     <t>SD Card Slot</t>
   </si>
   <si>
-    <t xml:space="preserve">798-DM3BT-DSF-PEJS </t>
+    <t xml:space="preserve">798-DM3CSSF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">640-USB4085-GF-A </t>
+  </si>
+  <si>
+    <t>USB C Buchse</t>
   </si>
 </sst>
 </file>
@@ -482,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AF3DBB-0668-B84A-B00B-44B9FC9FC66A}">
-  <dimension ref="A8:D27"/>
+  <dimension ref="A8:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -668,6 +674,17 @@
         <v>32</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pinout mit Viktor abgesprochen.
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\voltagerecorder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825BED41-6194-47D4-9084-B4BB65EFBD9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970DA84B-A475-4888-A345-00871B795CA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2090" windowWidth="21600" windowHeight="11470" xr2:uid="{48E2811D-28A7-1949-BAB9-61FD3C46DFFE}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="16200" windowHeight="9983" xr2:uid="{48E2811D-28A7-1949-BAB9-61FD3C46DFFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Anzahl</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>Trafo 2*115V, 2*14V</t>
+  </si>
+  <si>
+    <t>TVS Diode 3.3V SOD323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863-ESD7351HT1G </t>
+  </si>
+  <si>
+    <t>TVS Diode 5V SOD323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">833-ESD5V0D3-TP </t>
   </si>
 </sst>
 </file>
@@ -512,7 +524,7 @@
   <dimension ref="A8:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -728,6 +740,22 @@
         <v>38</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Packages zugeordnet, bom ergänzt.
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\voltagerecorder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970DA84B-A475-4888-A345-00871B795CA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47E28BD-ECA3-49F5-943B-9AF157BE7C66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1470" windowWidth="16200" windowHeight="9983" xr2:uid="{48E2811D-28A7-1949-BAB9-61FD3C46DFFE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Anzahl</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t xml:space="preserve">833-ESD5V0D3-TP </t>
+  </si>
+  <si>
+    <t>Taster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">611-PTS636SM25JSMTRL </t>
+  </si>
+  <si>
+    <t>Knopfzellenhalter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">534-500 </t>
   </si>
 </sst>
 </file>
@@ -521,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AF3DBB-0668-B84A-B00B-44B9FC9FC66A}">
-  <dimension ref="A8:D38"/>
+  <dimension ref="A8:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -756,22 +768,44 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A37" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A48" t="s">
         <v>39</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D48" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A38">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A49">
         <v>2</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B49" t="s">
         <v>41</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D49" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
G4 entfernt, I2C EEPROM hinzugefügt
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\voltagerecorder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47E28BD-ECA3-49F5-943B-9AF157BE7C66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BBF7F9-84DE-45F5-84CE-63D481B1270C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="16200" windowHeight="9983" xr2:uid="{48E2811D-28A7-1949-BAB9-61FD3C46DFFE}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="16201" windowHeight="9983" xr2:uid="{48E2811D-28A7-1949-BAB9-61FD3C46DFFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Anzahl</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t xml:space="preserve">534-500 </t>
+  </si>
+  <si>
+    <t>EEPROM 8k SOT-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">556-AT24CS08-STUM-T </t>
   </si>
 </sst>
 </file>
@@ -536,7 +542,7 @@
   <dimension ref="A8:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -790,6 +796,17 @@
         <v>49</v>
       </c>
     </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
         <v>39</v>

</xml_diff>